<commit_message>
Updated files to hide numpy warning. Redid tests and updated results accordingly. Updated notebook explanations accoring to review feedback
</commit_message>
<xml_diff>
--- a/Sign-Language-Recogniser/Results-graph.xlsx
+++ b/Sign-Language-Recogniser/Results-graph.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daniel/Projects/Udacity-AI/Sign-Language-Recogniser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.meechanibm.com/Code/Python/AI-Nanodegree/Sign-Language-Recogniser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -544,7 +544,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.57</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.65</c:v>
@@ -569,11 +569,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="685435136"/>
-        <c:axId val="685532688"/>
+        <c:axId val="-2078553296"/>
+        <c:axId val="-2078550464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="685435136"/>
+        <c:axId val="-2078553296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +616,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="685532688"/>
+        <c:crossAx val="-2078550464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="685532688"/>
+        <c:axId val="-2078550464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="685435136"/>
+        <c:crossAx val="-2078553296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,7 +1631,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D2">
-        <v>0.56999999999999995</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>